<commit_message>
Update the variable info
</commit_message>
<xml_diff>
--- a/etc/variables.xlsx
+++ b/etc/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrafaie/git/research/CTRNN/mems_ctrnn/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1FFDE673-C54B-E34E-B80D-D0E619B167EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C944C93D-C54B-A94D-B09B-EE99E264CD9D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,7 +211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -633,11 +633,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
@@ -647,7 +647,7 @@
     <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="32">
+    <row r="2" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -674,7 +674,7 @@
       </c>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
@@ -694,7 +694,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
@@ -714,7 +714,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
@@ -734,7 +734,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
@@ -754,7 +754,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
@@ -792,7 +792,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
@@ -810,7 +810,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
@@ -828,7 +828,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
@@ -848,7 +848,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>32</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
@@ -891,7 +891,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>38</v>
       </c>
@@ -907,7 +907,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>39</v>
       </c>
@@ -929,7 +929,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>40</v>
       </c>
@@ -953,7 +953,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>41</v>
       </c>
@@ -975,7 +975,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>43</v>
       </c>
@@ -991,7 +991,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
@@ -1007,7 +1007,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>56</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>57</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
         <v>58</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
         <v>59</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>

</xml_diff>